<commit_message>
Update daily benchmark data for May 30
</commit_message>
<xml_diff>
--- a/HenryHub_Daily.xlsx
+++ b/HenryHub_Daily.xlsx
@@ -32,7 +32,7 @@
     <t>This data may be copyrighted. Please refer to the Terms of Use: https://fred.stlouisfed.org/legal#fred-terms-faq</t>
   </si>
   <si>
-    <t>File Created: 2025-05-29 11:59 am CDT</t>
+    <t>File Created: 2025-05-30 9:04 am CDT</t>
   </si>
   <si>
     <t>DHHNGSP</t>
@@ -41,7 +41,7 @@
     <t>Henry Hub Natural Gas Spot Price, Dollars per Million BTU, Daily, Not Seasonally Adjusted</t>
   </si>
   <si>
-    <t>Data Updated: 2025-05-21</t>
+    <t>Data Updated: 2025-05-29</t>
   </si>
   <si>
     <t>observation_date</t>
@@ -490,278 +490,281 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4">
-        <v>45432</v>
+        <v>45440</v>
       </c>
       <c r="B2" s="2">
-        <v>2.52</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4">
-        <v>45433</v>
+        <v>45441</v>
       </c>
       <c r="B3" s="2">
-        <v>2.52</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4">
-        <v>45434</v>
+        <v>45442</v>
       </c>
       <c r="B4" s="2">
-        <v>2.51</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4">
-        <v>45435</v>
+        <v>45443</v>
       </c>
       <c r="B5" s="2">
-        <v>2.64</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4">
-        <v>45436</v>
+        <v>45446</v>
       </c>
       <c r="B6" s="2">
-        <v>2.22</v>
+        <v>2.55</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="4">
-        <v>45439</v>
+        <v>45447</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.58</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4">
-        <v>45440</v>
+        <v>45448</v>
       </c>
       <c r="B8" s="2">
-        <v>2.29</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4">
-        <v>45441</v>
+        <v>45449</v>
       </c>
       <c r="B9" s="2">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4">
-        <v>45442</v>
+        <v>45450</v>
       </c>
       <c r="B10" s="2">
-        <v>1.87</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4">
-        <v>45443</v>
+        <v>45453</v>
       </c>
       <c r="B11" s="2">
-        <v>1.78</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="4">
-        <v>45446</v>
+        <v>45454</v>
       </c>
       <c r="B12" s="2">
-        <v>2.55</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="4">
-        <v>45447</v>
+        <v>45455</v>
       </c>
       <c r="B13" s="2">
-        <v>2.58</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="4">
-        <v>45448</v>
+        <v>45456</v>
       </c>
       <c r="B14" s="2">
-        <v>2.27</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="4">
-        <v>45449</v>
+        <v>45457</v>
       </c>
       <c r="B15" s="2">
-        <v>2.3</v>
+        <v>2.74</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="4">
-        <v>45450</v>
+        <v>45460</v>
       </c>
       <c r="B16" s="2">
-        <v>2.46</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4">
-        <v>45453</v>
+        <v>45461</v>
       </c>
       <c r="B17" s="2">
-        <v>2.61</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="4">
-        <v>45454</v>
-      </c>
-      <c r="B18" s="2">
-        <v>2.71</v>
+        <v>45462</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="4">
-        <v>45455</v>
+        <v>45463</v>
       </c>
       <c r="B19" s="2">
-        <v>2.8</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="4">
-        <v>45456</v>
+        <v>45464</v>
       </c>
       <c r="B20" s="2">
-        <v>2.79</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="4">
-        <v>45457</v>
+        <v>45467</v>
       </c>
       <c r="B21" s="2">
-        <v>2.74</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="4">
-        <v>45460</v>
+        <v>45468</v>
       </c>
       <c r="B22" s="2">
-        <v>2.5</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="4">
-        <v>45461</v>
+        <v>45469</v>
       </c>
       <c r="B23" s="2">
-        <v>2.43</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="4">
-        <v>45462</v>
+        <v>45470</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2.55</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="4">
-        <v>45463</v>
+        <v>45471</v>
       </c>
       <c r="B25" s="2">
-        <v>2.39</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="4">
-        <v>45464</v>
+        <v>45474</v>
       </c>
       <c r="B26" s="2">
-        <v>2.44</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="4">
-        <v>45467</v>
+        <v>45475</v>
       </c>
       <c r="B27" s="2">
-        <v>2.58</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="4">
-        <v>45468</v>
+        <v>45476</v>
       </c>
       <c r="B28" s="2">
-        <v>2.61</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="4">
-        <v>45469</v>
-      </c>
-      <c r="B29" s="2">
-        <v>2.45</v>
+        <v>45477</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4">
-        <v>45470</v>
+        <v>45478</v>
       </c>
       <c r="B30" s="2">
-        <v>2.55</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="4">
-        <v>45471</v>
+        <v>45481</v>
       </c>
       <c r="B31" s="2">
-        <v>2.42</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="4">
-        <v>45474</v>
+        <v>45482</v>
       </c>
       <c r="B32" s="2">
-        <v>2.21</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="4">
-        <v>45475</v>
+        <v>45483</v>
       </c>
       <c r="B33" s="2">
-        <v>2.06</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="4">
-        <v>45476</v>
+        <v>45484</v>
       </c>
       <c r="B34" s="2">
-        <v>2.02</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="4">
-        <v>45477</v>
+        <v>45485</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2.17</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="4">
-        <v>45478</v>
+        <v>45488</v>
       </c>
       <c r="B36" s="2">
-        <v>2.02</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="4">
-        <v>45481</v>
+        <v>45489</v>
       </c>
       <c r="B37" s="2">
         <v>2.1</v>
@@ -769,263 +772,263 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="4">
-        <v>45482</v>
+        <v>45490</v>
       </c>
       <c r="B38" s="2">
-        <v>2.42</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="4">
-        <v>45483</v>
+        <v>45491</v>
       </c>
       <c r="B39" s="2">
-        <v>2.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="4">
-        <v>45484</v>
+        <v>45492</v>
       </c>
       <c r="B40" s="2">
-        <v>2.23</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="4">
-        <v>45485</v>
+        <v>45495</v>
       </c>
       <c r="B41" s="2">
-        <v>2.17</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="4">
-        <v>45488</v>
+        <v>45496</v>
       </c>
       <c r="B42" s="2">
-        <v>2.12</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="4">
-        <v>45489</v>
+        <v>45497</v>
       </c>
       <c r="B43" s="2">
-        <v>2.1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="4">
-        <v>45490</v>
+        <v>45498</v>
       </c>
       <c r="B44" s="2">
-        <v>1.98</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="4">
-        <v>45491</v>
+        <v>45499</v>
       </c>
       <c r="B45" s="2">
-        <v>2</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="4">
-        <v>45492</v>
+        <v>45502</v>
       </c>
       <c r="B46" s="2">
-        <v>1.88</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="4">
-        <v>45495</v>
+        <v>45503</v>
       </c>
       <c r="B47" s="2">
-        <v>2.19</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="4">
-        <v>45496</v>
+        <v>45504</v>
       </c>
       <c r="B48" s="2">
-        <v>2.13</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="4">
-        <v>45497</v>
+        <v>45505</v>
       </c>
       <c r="B49" s="2">
-        <v>2</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="4">
-        <v>45498</v>
+        <v>45506</v>
       </c>
       <c r="B50" s="2">
-        <v>2</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="4">
-        <v>45499</v>
+        <v>45509</v>
       </c>
       <c r="B51" s="2">
-        <v>1.98</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="4">
-        <v>45502</v>
+        <v>45510</v>
       </c>
       <c r="B52" s="2">
-        <v>1.9</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="4">
-        <v>45503</v>
+        <v>45511</v>
       </c>
       <c r="B53" s="2">
-        <v>1.81</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="4">
-        <v>45504</v>
+        <v>45512</v>
       </c>
       <c r="B54" s="2">
-        <v>1.94</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="4">
-        <v>45505</v>
+        <v>45513</v>
       </c>
       <c r="B55" s="2">
-        <v>1.95</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="4">
-        <v>45506</v>
+        <v>45516</v>
       </c>
       <c r="B56" s="2">
-        <v>1.89</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="4">
-        <v>45509</v>
+        <v>45517</v>
       </c>
       <c r="B57" s="2">
-        <v>1.83</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="4">
-        <v>45510</v>
+        <v>45518</v>
       </c>
       <c r="B58" s="2">
-        <v>1.83</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="4">
-        <v>45511</v>
+        <v>45519</v>
       </c>
       <c r="B59" s="2">
-        <v>1.96</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="4">
-        <v>45512</v>
+        <v>45520</v>
       </c>
       <c r="B60" s="2">
-        <v>1.85</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="4">
-        <v>45513</v>
+        <v>45523</v>
       </c>
       <c r="B61" s="2">
-        <v>1.94</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="4">
-        <v>45516</v>
+        <v>45524</v>
       </c>
       <c r="B62" s="2">
-        <v>2.1</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="4">
-        <v>45517</v>
+        <v>45525</v>
       </c>
       <c r="B63" s="2">
-        <v>2.16</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="4">
-        <v>45518</v>
+        <v>45526</v>
       </c>
       <c r="B64" s="2">
-        <v>2.18</v>
+        <v>1.93</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="4">
-        <v>45519</v>
+        <v>45527</v>
       </c>
       <c r="B65" s="2">
-        <v>2.19</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="4">
-        <v>45520</v>
+        <v>45530</v>
       </c>
       <c r="B66" s="2">
-        <v>2.01</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="4">
-        <v>45523</v>
+        <v>45531</v>
       </c>
       <c r="B67" s="2">
-        <v>2.12</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="4">
-        <v>45524</v>
+        <v>45532</v>
       </c>
       <c r="B68" s="2">
-        <v>2.18</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="4">
-        <v>45525</v>
+        <v>45533</v>
       </c>
       <c r="B69" s="2">
-        <v>2.14</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="4">
-        <v>45526</v>
+        <v>45534</v>
       </c>
       <c r="B70" s="2">
         <v>1.93</v>
@@ -1033,800 +1036,797 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="4">
-        <v>45527</v>
-      </c>
-      <c r="B71" s="2">
-        <v>1.82</v>
+        <v>45537</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="4">
-        <v>45530</v>
+        <v>45538</v>
       </c>
       <c r="B72" s="2">
-        <v>2.13</v>
+        <v>1.93</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="4">
-        <v>45531</v>
+        <v>45539</v>
       </c>
       <c r="B73" s="2">
-        <v>1.91</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="4">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B74" s="2">
-        <v>1.89</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="4">
-        <v>45533</v>
+        <v>45541</v>
       </c>
       <c r="B75" s="2">
-        <v>1.85</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="4">
-        <v>45534</v>
+        <v>45544</v>
       </c>
       <c r="B76" s="2">
-        <v>1.93</v>
+        <v>2.03</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="4">
-        <v>45537</v>
+        <v>45545</v>
+      </c>
+      <c r="B77" s="2">
+        <v>2.13</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="4">
-        <v>45538</v>
+        <v>45546</v>
       </c>
       <c r="B78" s="2">
-        <v>1.93</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="4">
-        <v>45539</v>
+        <v>45547</v>
       </c>
       <c r="B79" s="2">
-        <v>2.05</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="4">
-        <v>45540</v>
+        <v>45548</v>
       </c>
       <c r="B80" s="2">
-        <v>2.02</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="4">
-        <v>45541</v>
+        <v>45551</v>
       </c>
       <c r="B81" s="2">
-        <v>2.09</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="4">
-        <v>45544</v>
+        <v>45552</v>
       </c>
       <c r="B82" s="2">
-        <v>2.03</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="4">
-        <v>45545</v>
+        <v>45553</v>
       </c>
       <c r="B83" s="2">
-        <v>2.13</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="4">
-        <v>45546</v>
+        <v>45554</v>
       </c>
       <c r="B84" s="2">
-        <v>2.13</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="4">
-        <v>45547</v>
+        <v>45555</v>
       </c>
       <c r="B85" s="2">
-        <v>2.13</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="4">
-        <v>45548</v>
+        <v>45558</v>
       </c>
       <c r="B86" s="2">
-        <v>2.25</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="4">
-        <v>45551</v>
+        <v>45559</v>
       </c>
       <c r="B87" s="2">
-        <v>2.23</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="4">
-        <v>45552</v>
+        <v>45560</v>
       </c>
       <c r="B88" s="2">
-        <v>2.33</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="4">
-        <v>45553</v>
+        <v>45561</v>
       </c>
       <c r="B89" s="2">
-        <v>2.31</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="4">
-        <v>45554</v>
+        <v>45562</v>
       </c>
       <c r="B90" s="2">
-        <v>2.24</v>
+        <v>2.53</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="4">
-        <v>45555</v>
+        <v>45565</v>
       </c>
       <c r="B91" s="2">
-        <v>2.2</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="4">
-        <v>45558</v>
+        <v>45566</v>
       </c>
       <c r="B92" s="2">
-        <v>2.4</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="4">
-        <v>45559</v>
+        <v>45567</v>
       </c>
       <c r="B93" s="2">
-        <v>2.61</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="4">
-        <v>45560</v>
+        <v>45568</v>
       </c>
       <c r="B94" s="2">
-        <v>2.62</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="4">
-        <v>45561</v>
+        <v>45569</v>
       </c>
       <c r="B95" s="2">
-        <v>2.64</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="4">
-        <v>45562</v>
+        <v>45572</v>
       </c>
       <c r="B96" s="2">
-        <v>2.53</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="4">
-        <v>45565</v>
+        <v>45573</v>
       </c>
       <c r="B97" s="2">
-        <v>2.65</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="4">
-        <v>45566</v>
+        <v>45574</v>
       </c>
       <c r="B98" s="2">
-        <v>2.67</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="4">
-        <v>45567</v>
+        <v>45575</v>
       </c>
       <c r="B99" s="2">
-        <v>2.77</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="4">
-        <v>45568</v>
+        <v>45576</v>
       </c>
       <c r="B100" s="2">
-        <v>2.75</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="4">
-        <v>45569</v>
-      </c>
-      <c r="B101" s="2">
-        <v>2.49</v>
+        <v>45579</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="4">
-        <v>45572</v>
+        <v>45580</v>
       </c>
       <c r="B102" s="2">
-        <v>2.51</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="4">
-        <v>45573</v>
+        <v>45581</v>
       </c>
       <c r="B103" s="2">
-        <v>2.51</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="4">
-        <v>45574</v>
+        <v>45582</v>
       </c>
       <c r="B104" s="2">
-        <v>2.43</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="4">
-        <v>45575</v>
+        <v>45583</v>
       </c>
       <c r="B105" s="2">
-        <v>2.26</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="4">
-        <v>45576</v>
+        <v>45586</v>
       </c>
       <c r="B106" s="2">
-        <v>2.31</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="4">
-        <v>45579</v>
+        <v>45587</v>
+      </c>
+      <c r="B107" s="2">
+        <v>1.76</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="4">
-        <v>45580</v>
+        <v>45588</v>
       </c>
       <c r="B108" s="2">
-        <v>2.37</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="4">
-        <v>45581</v>
+        <v>45589</v>
       </c>
       <c r="B109" s="2">
-        <v>2.21</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="4">
-        <v>45582</v>
+        <v>45590</v>
       </c>
       <c r="B110" s="2">
-        <v>2.19</v>
+        <v>1.93</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="4">
-        <v>45583</v>
+        <v>45593</v>
       </c>
       <c r="B111" s="2">
-        <v>1.82</v>
+        <v>2.03</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="4">
-        <v>45586</v>
+        <v>45594</v>
       </c>
       <c r="B112" s="2">
-        <v>1.76</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="4">
-        <v>45587</v>
+        <v>45595</v>
       </c>
       <c r="B113" s="2">
-        <v>1.76</v>
+        <v>2.03</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="4">
-        <v>45588</v>
+        <v>45596</v>
       </c>
       <c r="B114" s="2">
-        <v>1.9</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="4">
-        <v>45589</v>
+        <v>45597</v>
       </c>
       <c r="B115" s="2">
-        <v>2.04</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="4">
-        <v>45590</v>
+        <v>45600</v>
       </c>
       <c r="B116" s="2">
-        <v>1.93</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="4">
-        <v>45593</v>
+        <v>45601</v>
       </c>
       <c r="B117" s="2">
-        <v>2.03</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="4">
-        <v>45594</v>
+        <v>45602</v>
       </c>
       <c r="B118" s="2">
-        <v>1.82</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="4">
-        <v>45595</v>
+        <v>45603</v>
       </c>
       <c r="B119" s="2">
-        <v>2.03</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="4">
-        <v>45596</v>
+        <v>45604</v>
       </c>
       <c r="B120" s="2">
-        <v>1.82</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="4">
-        <v>45597</v>
+        <v>45607</v>
       </c>
       <c r="B121" s="2">
-        <v>1.42</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="4">
-        <v>45600</v>
+        <v>45608</v>
       </c>
       <c r="B122" s="2">
-        <v>1.35</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="4">
-        <v>45601</v>
+        <v>45609</v>
       </c>
       <c r="B123" s="2">
-        <v>1.62</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="4">
-        <v>45602</v>
+        <v>45610</v>
       </c>
       <c r="B124" s="2">
-        <v>1.8</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="4">
-        <v>45603</v>
+        <v>45611</v>
       </c>
       <c r="B125" s="2">
-        <v>1.49</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="4">
-        <v>45604</v>
+        <v>45614</v>
       </c>
       <c r="B126" s="2">
-        <v>1.21</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="4">
-        <v>45607</v>
+        <v>45615</v>
       </c>
       <c r="B127" s="2">
-        <v>1.21</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="4">
-        <v>45608</v>
+        <v>45616</v>
       </c>
       <c r="B128" s="2">
-        <v>1.92</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="4">
-        <v>45609</v>
+        <v>45617</v>
       </c>
       <c r="B129" s="2">
-        <v>2.06</v>
+        <v>2.84</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="4">
-        <v>45610</v>
+        <v>45618</v>
       </c>
       <c r="B130" s="2">
-        <v>2.11</v>
+        <v>2.41</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="4">
-        <v>45611</v>
+        <v>45621</v>
       </c>
       <c r="B131" s="2">
-        <v>1.65</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="4">
-        <v>45614</v>
+        <v>45622</v>
       </c>
       <c r="B132" s="2">
-        <v>2.08</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="4">
-        <v>45615</v>
+        <v>45623</v>
       </c>
       <c r="B133" s="2">
-        <v>2.1</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="4">
-        <v>45616</v>
-      </c>
-      <c r="B134" s="2">
-        <v>2.32</v>
+        <v>45624</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="4">
-        <v>45617</v>
+        <v>45625</v>
       </c>
       <c r="B135" s="2">
-        <v>2.84</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="4">
-        <v>45618</v>
+        <v>45628</v>
       </c>
       <c r="B136" s="2">
-        <v>2.41</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="4">
-        <v>45621</v>
+        <v>45629</v>
       </c>
       <c r="B137" s="2">
-        <v>2.78</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="4">
-        <v>45622</v>
+        <v>45630</v>
       </c>
       <c r="B138" s="2">
-        <v>3.19</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="4">
-        <v>45623</v>
+        <v>45631</v>
       </c>
       <c r="B139" s="2">
-        <v>3.39</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="4">
-        <v>45624</v>
+        <v>45632</v>
+      </c>
+      <c r="B140" s="2">
+        <v>2.83</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="4">
-        <v>45625</v>
+        <v>45635</v>
       </c>
       <c r="B141" s="2">
-        <v>3.39</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="4">
-        <v>45628</v>
+        <v>45636</v>
       </c>
       <c r="B142" s="2">
-        <v>3.05</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="4">
-        <v>45629</v>
+        <v>45637</v>
       </c>
       <c r="B143" s="2">
-        <v>2.94</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="4">
-        <v>45630</v>
+        <v>45638</v>
       </c>
       <c r="B144" s="2">
-        <v>2.75</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="4">
-        <v>45631</v>
+        <v>45639</v>
       </c>
       <c r="B145" s="2">
-        <v>2.95</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="4">
-        <v>45632</v>
+        <v>45642</v>
       </c>
       <c r="B146" s="2">
-        <v>2.83</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="4">
-        <v>45635</v>
+        <v>45643</v>
       </c>
       <c r="B147" s="2">
-        <v>3.05</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="4">
-        <v>45636</v>
+        <v>45644</v>
       </c>
       <c r="B148" s="2">
-        <v>2.9</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="4">
-        <v>45637</v>
+        <v>45645</v>
       </c>
       <c r="B149" s="2">
-        <v>2.9</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="4">
-        <v>45638</v>
+        <v>45646</v>
       </c>
       <c r="B150" s="2">
-        <v>3.12</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="4">
-        <v>45639</v>
+        <v>45649</v>
       </c>
       <c r="B151" s="2">
-        <v>3.15</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="4">
-        <v>45642</v>
+        <v>45650</v>
       </c>
       <c r="B152" s="2">
-        <v>2.87</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="4">
-        <v>45643</v>
-      </c>
-      <c r="B153" s="2">
-        <v>2.85</v>
+        <v>45651</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="4">
-        <v>45644</v>
+        <v>45652</v>
       </c>
       <c r="B154" s="2">
-        <v>3.01</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="4">
-        <v>45645</v>
+        <v>45653</v>
       </c>
       <c r="B155" s="2">
-        <v>3.15</v>
+        <v>2.91</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="4">
-        <v>45646</v>
+        <v>45656</v>
       </c>
       <c r="B156" s="2">
-        <v>3.1</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="4">
-        <v>45649</v>
+        <v>45657</v>
       </c>
       <c r="B157" s="2">
-        <v>2.89</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="4">
-        <v>45650</v>
-      </c>
-      <c r="B158" s="2">
-        <v>2.95</v>
+        <v>45658</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="4">
-        <v>45651</v>
+        <v>45659</v>
+      </c>
+      <c r="B159" s="2">
+        <v>3.65</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="4">
-        <v>45652</v>
+        <v>45660</v>
       </c>
       <c r="B160" s="2">
-        <v>2.96</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="4">
-        <v>45653</v>
+        <v>45663</v>
       </c>
       <c r="B161" s="2">
-        <v>2.91</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="4">
-        <v>45656</v>
+        <v>45664</v>
       </c>
       <c r="B162" s="2">
-        <v>3.39</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="4">
-        <v>45657</v>
+        <v>45665</v>
       </c>
       <c r="B163" s="2">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="4">
-        <v>45658</v>
+        <v>45666</v>
+      </c>
+      <c r="B164" s="2">
+        <v>3.94</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="4">
-        <v>45659</v>
+        <v>45667</v>
       </c>
       <c r="B165" s="2">
-        <v>3.65</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="4">
-        <v>45660</v>
+        <v>45670</v>
       </c>
       <c r="B166" s="2">
-        <v>3.4</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="4">
-        <v>45663</v>
+        <v>45671</v>
       </c>
       <c r="B167" s="2">
-        <v>4.05</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="4">
-        <v>45664</v>
+        <v>45672</v>
       </c>
       <c r="B168" s="2">
-        <v>3.8</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="4">
-        <v>45665</v>
+        <v>45673</v>
       </c>
       <c r="B169" s="2">
-        <v>3.75</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="4">
-        <v>45666</v>
+        <v>45674</v>
       </c>
       <c r="B170" s="2">
-        <v>3.94</v>
+        <v>9.859999999999999</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="4">
-        <v>45667</v>
-      </c>
-      <c r="B171" s="2">
-        <v>4.13</v>
+        <v>45677</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="4">
-        <v>45670</v>
+        <v>45678</v>
       </c>
       <c r="B172" s="2">
         <v>4.4</v>
@@ -1834,180 +1834,180 @@
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="4">
-        <v>45671</v>
+        <v>45679</v>
       </c>
       <c r="B173" s="2">
-        <v>4.32</v>
+        <v>3.91</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="4">
-        <v>45672</v>
+        <v>45680</v>
       </c>
       <c r="B174" s="2">
-        <v>4.45</v>
+        <v>3.91</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="4">
-        <v>45673</v>
+        <v>45681</v>
       </c>
       <c r="B175" s="2">
-        <v>4.3</v>
+        <v>3.84</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="4">
-        <v>45674</v>
+        <v>45684</v>
       </c>
       <c r="B176" s="2">
-        <v>9.859999999999999</v>
+        <v>3.71</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="4">
-        <v>45677</v>
+        <v>45685</v>
+      </c>
+      <c r="B177" s="2">
+        <v>3.4</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="4">
-        <v>45678</v>
+        <v>45686</v>
       </c>
       <c r="B178" s="2">
-        <v>4.4</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="4">
-        <v>45679</v>
+        <v>45687</v>
       </c>
       <c r="B179" s="2">
-        <v>3.91</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="4">
-        <v>45680</v>
+        <v>45688</v>
       </c>
       <c r="B180" s="2">
-        <v>3.91</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="4">
-        <v>45681</v>
+        <v>45691</v>
       </c>
       <c r="B181" s="2">
-        <v>3.84</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="4">
-        <v>45684</v>
+        <v>45692</v>
       </c>
       <c r="B182" s="2">
-        <v>3.71</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="4">
-        <v>45685</v>
+        <v>45693</v>
       </c>
       <c r="B183" s="2">
-        <v>3.4</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="4">
-        <v>45686</v>
+        <v>45694</v>
       </c>
       <c r="B184" s="2">
-        <v>3.38</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="4">
-        <v>45687</v>
+        <v>45695</v>
       </c>
       <c r="B185" s="2">
-        <v>3.12</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="4">
-        <v>45688</v>
+        <v>45698</v>
       </c>
       <c r="B186" s="2">
-        <v>2.93</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="4">
-        <v>45691</v>
+        <v>45699</v>
       </c>
       <c r="B187" s="2">
-        <v>3.3</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="4">
-        <v>45692</v>
+        <v>45700</v>
       </c>
       <c r="B188" s="2">
-        <v>3.25</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="4">
-        <v>45693</v>
+        <v>45701</v>
       </c>
       <c r="B189" s="2">
-        <v>3.22</v>
+        <v>4.43</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="4">
-        <v>45694</v>
+        <v>45702</v>
       </c>
       <c r="B190" s="2">
-        <v>3.31</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="4">
-        <v>45695</v>
-      </c>
-      <c r="B191" s="2">
-        <v>3.32</v>
+        <v>45705</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="4">
-        <v>45698</v>
+        <v>45706</v>
       </c>
       <c r="B192" s="2">
-        <v>3.48</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="4">
-        <v>45699</v>
+        <v>45707</v>
       </c>
       <c r="B193" s="2">
-        <v>3.65</v>
+        <v>7.15</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="4">
-        <v>45700</v>
+        <v>45708</v>
       </c>
       <c r="B194" s="2">
-        <v>3.97</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="4">
-        <v>45701</v>
+        <v>45709</v>
       </c>
       <c r="B195" s="2">
         <v>4.43</v>
@@ -2015,377 +2015,380 @@
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="4">
-        <v>45702</v>
+        <v>45712</v>
       </c>
       <c r="B196" s="2">
-        <v>4.6</v>
+        <v>3.86</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="4">
-        <v>45705</v>
+        <v>45713</v>
+      </c>
+      <c r="B197" s="2">
+        <v>3.88</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="4">
-        <v>45706</v>
+        <v>45714</v>
       </c>
       <c r="B198" s="2">
-        <v>6.4</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="4">
-        <v>45707</v>
+        <v>45715</v>
       </c>
       <c r="B199" s="2">
-        <v>7.15</v>
+        <v>3.91</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="4">
-        <v>45708</v>
+        <v>45716</v>
       </c>
       <c r="B200" s="2">
-        <v>5.62</v>
+        <v>3.91</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="4">
-        <v>45709</v>
+        <v>45719</v>
       </c>
       <c r="B201" s="2">
-        <v>4.43</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="4">
-        <v>45712</v>
+        <v>45720</v>
       </c>
       <c r="B202" s="2">
-        <v>3.86</v>
+        <v>4.39</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="4">
-        <v>45713</v>
+        <v>45721</v>
       </c>
       <c r="B203" s="2">
-        <v>3.88</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="4">
-        <v>45714</v>
+        <v>45722</v>
       </c>
       <c r="B204" s="2">
-        <v>3.9</v>
+        <v>4.39</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="4">
-        <v>45715</v>
+        <v>45723</v>
       </c>
       <c r="B205" s="2">
-        <v>3.91</v>
+        <v>4.39</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="4">
-        <v>45716</v>
+        <v>45726</v>
       </c>
       <c r="B206" s="2">
-        <v>3.91</v>
+        <v>4.23</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="4">
-        <v>45719</v>
+        <v>45727</v>
       </c>
       <c r="B207" s="2">
-        <v>3.8</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="4">
-        <v>45720</v>
+        <v>45728</v>
       </c>
       <c r="B208" s="2">
-        <v>4.39</v>
+        <v>4.18</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="4">
-        <v>45721</v>
+        <v>45729</v>
       </c>
       <c r="B209" s="2">
-        <v>4.4</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="4">
-        <v>45722</v>
+        <v>45730</v>
       </c>
       <c r="B210" s="2">
-        <v>4.39</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="4">
-        <v>45723</v>
+        <v>45733</v>
       </c>
       <c r="B211" s="2">
-        <v>4.39</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="4">
-        <v>45726</v>
+        <v>45734</v>
       </c>
       <c r="B212" s="2">
-        <v>4.23</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="4">
-        <v>45727</v>
+        <v>45735</v>
       </c>
       <c r="B213" s="2">
-        <v>4.57</v>
+        <v>4.21</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="4">
-        <v>45728</v>
+        <v>45736</v>
       </c>
       <c r="B214" s="2">
-        <v>4.18</v>
+        <v>4.23</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="4">
-        <v>45729</v>
+        <v>45737</v>
       </c>
       <c r="B215" s="2">
-        <v>3.89</v>
+        <v>3.93</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="4">
-        <v>45730</v>
+        <v>45740</v>
       </c>
       <c r="B216" s="2">
-        <v>3.89</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="4">
-        <v>45733</v>
+        <v>45741</v>
       </c>
       <c r="B217" s="2">
-        <v>4.15</v>
+        <v>3.94</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="4">
-        <v>45734</v>
+        <v>45742</v>
       </c>
       <c r="B218" s="2">
-        <v>4.17</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="4">
-        <v>45735</v>
+        <v>45743</v>
       </c>
       <c r="B219" s="2">
-        <v>4.21</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="4">
-        <v>45736</v>
+        <v>45744</v>
       </c>
       <c r="B220" s="2">
-        <v>4.23</v>
+        <v>3.89</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" s="4">
-        <v>45737</v>
+        <v>45747</v>
       </c>
       <c r="B221" s="2">
-        <v>3.93</v>
+        <v>4.11</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="4">
-        <v>45740</v>
+        <v>45748</v>
       </c>
       <c r="B222" s="2">
-        <v>4.03</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="4">
-        <v>45741</v>
+        <v>45749</v>
       </c>
       <c r="B223" s="2">
-        <v>3.94</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="4">
-        <v>45742</v>
+        <v>45750</v>
       </c>
       <c r="B224" s="2">
-        <v>3.85</v>
+        <v>4.21</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="4">
-        <v>45743</v>
+        <v>45751</v>
       </c>
       <c r="B225" s="2">
-        <v>3.88</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="4">
-        <v>45744</v>
+        <v>45754</v>
       </c>
       <c r="B226" s="2">
-        <v>3.89</v>
+        <v>3.97</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="4">
-        <v>45747</v>
+        <v>45755</v>
       </c>
       <c r="B227" s="2">
-        <v>4.11</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="4">
-        <v>45748</v>
+        <v>45756</v>
       </c>
       <c r="B228" s="2">
-        <v>3.96</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="4">
-        <v>45749</v>
+        <v>45757</v>
       </c>
       <c r="B229" s="2">
-        <v>4.04</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="4">
-        <v>45750</v>
+        <v>45758</v>
       </c>
       <c r="B230" s="2">
-        <v>4.21</v>
+        <v>3.44</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="4">
-        <v>45751</v>
+        <v>45761</v>
       </c>
       <c r="B231" s="2">
-        <v>4.04</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="4">
-        <v>45754</v>
+        <v>45762</v>
       </c>
       <c r="B232" s="2">
-        <v>3.97</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="4">
-        <v>45755</v>
+        <v>45763</v>
       </c>
       <c r="B233" s="2">
-        <v>3.85</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="4">
-        <v>45756</v>
+        <v>45764</v>
       </c>
       <c r="B234" s="2">
-        <v>3.42</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="4">
-        <v>45757</v>
-      </c>
-      <c r="B235" s="2">
-        <v>3.7</v>
+        <v>45765</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="4">
-        <v>45758</v>
+        <v>45768</v>
       </c>
       <c r="B236" s="2">
-        <v>3.44</v>
+        <v>3.16</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" s="4">
-        <v>45761</v>
+        <v>45769</v>
       </c>
       <c r="B237" s="2">
-        <v>3.57</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="4">
-        <v>45762</v>
+        <v>45770</v>
       </c>
       <c r="B238" s="2">
-        <v>3.27</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" s="4">
-        <v>45763</v>
+        <v>45771</v>
       </c>
       <c r="B239" s="2">
-        <v>3.25</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="4">
-        <v>45764</v>
+        <v>45772</v>
       </c>
       <c r="B240" s="2">
-        <v>2.94</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="4">
-        <v>45765</v>
+        <v>45775</v>
+      </c>
+      <c r="B241" s="2">
+        <v>2.96</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" s="4">
-        <v>45768</v>
+        <v>45776</v>
       </c>
       <c r="B242" s="2">
-        <v>3.16</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" s="4">
-        <v>45769</v>
+        <v>45777</v>
       </c>
       <c r="B243" s="2">
         <v>3.12</v>
@@ -2393,154 +2396,151 @@
     </row>
     <row r="244" spans="1:2">
       <c r="A244" s="4">
-        <v>45770</v>
+        <v>45778</v>
       </c>
       <c r="B244" s="2">
-        <v>3.12</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" s="4">
-        <v>45771</v>
+        <v>45779</v>
       </c>
       <c r="B245" s="2">
-        <v>2.87</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" s="4">
-        <v>45772</v>
+        <v>45782</v>
       </c>
       <c r="B246" s="2">
-        <v>2.71</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" s="4">
-        <v>45775</v>
+        <v>45783</v>
       </c>
       <c r="B247" s="2">
-        <v>2.96</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" s="4">
-        <v>45776</v>
+        <v>45784</v>
       </c>
       <c r="B248" s="2">
-        <v>3.17</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" s="4">
-        <v>45777</v>
+        <v>45785</v>
       </c>
       <c r="B249" s="2">
-        <v>3.12</v>
+        <v>3.23</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" s="4">
-        <v>45778</v>
+        <v>45786</v>
       </c>
       <c r="B250" s="2">
-        <v>3.08</v>
+        <v>3.22</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" s="4">
-        <v>45779</v>
+        <v>45789</v>
       </c>
       <c r="B251" s="2">
-        <v>3.1</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" s="4">
-        <v>45782</v>
+        <v>45790</v>
       </c>
       <c r="B252" s="2">
-        <v>3.26</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" s="4">
-        <v>45783</v>
+        <v>45791</v>
       </c>
       <c r="B253" s="2">
-        <v>3.08</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" s="4">
-        <v>45784</v>
+        <v>45792</v>
       </c>
       <c r="B254" s="2">
-        <v>3.18</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" s="4">
-        <v>45785</v>
+        <v>45793</v>
       </c>
       <c r="B255" s="2">
-        <v>3.23</v>
+        <v>3.01</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" s="4">
-        <v>45786</v>
+        <v>45796</v>
       </c>
       <c r="B256" s="2">
-        <v>3.22</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" s="4">
-        <v>45789</v>
+        <v>45797</v>
       </c>
       <c r="B257" s="2">
-        <v>3.19</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" s="4">
-        <v>45790</v>
+        <v>45798</v>
       </c>
       <c r="B258" s="2">
-        <v>3.27</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="4">
-        <v>45791</v>
+        <v>45799</v>
       </c>
       <c r="B259" s="2">
-        <v>3.31</v>
+        <v>3</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="4">
-        <v>45792</v>
+        <v>45800</v>
       </c>
       <c r="B260" s="2">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" s="4">
-        <v>45793</v>
-      </c>
-      <c r="B261" s="2">
-        <v>3.01</v>
+        <v>45803</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="4">
-        <v>45796</v>
+        <v>45804</v>
       </c>
       <c r="B262" s="2">
-        <v>2.96</v>
+        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>